<commit_message>
genism search: only nouns
</commit_message>
<xml_diff>
--- a/output/frat/conceptnet-local_embedding_search/depth_2/embeddings/frat_3_conceptnet_search_embeddings-top10.xlsx
+++ b/output/frat/conceptnet-local_embedding_search/depth_2/embeddings/frat_3_conceptnet_search_embeddings-top10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\r_m_thesis\output\frat\conceptnet-local_embedding_search\depth_2\embeddings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004A5A01-802D-4E48-A73B-FFF8DA62B41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05017F3F-50CD-4782-AF04-F03389050C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1385,7 +1385,7 @@
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="27.7265625" customWidth="1"/>
-    <col min="4" max="4" width="33.6328125" customWidth="1"/>
+    <col min="4" max="4" width="61.26953125" customWidth="1"/>
     <col min="5" max="5" width="29.81640625" customWidth="1"/>
     <col min="6" max="6" width="27.54296875" customWidth="1"/>
     <col min="7" max="7" width="43.7265625" customWidth="1"/>

</xml_diff>